<commit_message>
Updated Player Stats and Leveling
- Updated player stats struct and CSV to implement used variables, and to remove unused ones

- Added player levelling which now determines player health and armor from dice rolls
</commit_message>
<xml_diff>
--- a/datafiles/player_data.xlsx
+++ b/datafiles/player_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -25,21 +25,6 @@
     <t>Seki</t>
   </si>
   <si>
-    <t>HP</t>
-  </si>
-  <si>
-    <t>Armor</t>
-  </si>
-  <si>
-    <t>Movement Speed</t>
-  </si>
-  <si>
-    <t>Main Attack Speed</t>
-  </si>
-  <si>
-    <t>Main Attack Damage</t>
-  </si>
-  <si>
     <t>Xan</t>
   </si>
   <si>
@@ -59,6 +44,24 @@
   </si>
   <si>
     <t>Nyx</t>
+  </si>
+  <si>
+    <t>dice_hp</t>
+  </si>
+  <si>
+    <t>dice_armor</t>
+  </si>
+  <si>
+    <t>move_spd</t>
+  </si>
+  <si>
+    <t>main_atk_spd</t>
+  </si>
+  <si>
+    <t>hp_mod</t>
+  </si>
+  <si>
+    <t>view_range</t>
   </si>
 </sst>
 </file>
@@ -82,7 +85,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -90,12 +93,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,224 +440,296 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G9"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="H2" s="2">
+        <v>250</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E3" s="2">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="H3" s="2">
+        <v>250</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="H4" s="2">
+        <v>250</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B5" s="2">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="H5" s="2">
+        <v>250</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="H6" s="2">
+        <v>250</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B7" s="2">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="E7" s="2">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="H7" s="2">
+        <v>250</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="H8" s="2">
+        <v>250</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>100</v>
-      </c>
-      <c r="C2">
-        <v>80</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <v>20</v>
-      </c>
-      <c r="F2">
+      <c r="B9" s="2">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2">
         <v>0.25</v>
       </c>
-      <c r="G2">
+      <c r="G9" s="2">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>60</v>
-      </c>
-      <c r="C3">
-        <v>20</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <v>0.25</v>
-      </c>
-      <c r="G3">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>80</v>
-      </c>
-      <c r="C4">
-        <v>35</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>0.25</v>
-      </c>
-      <c r="G4">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>110</v>
-      </c>
-      <c r="C5">
-        <v>50</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>15</v>
-      </c>
-      <c r="F5">
-        <v>0.25</v>
-      </c>
-      <c r="G5">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>90</v>
-      </c>
-      <c r="C6">
-        <v>30</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6">
-        <v>0.25</v>
-      </c>
-      <c r="G6">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>130</v>
-      </c>
-      <c r="C7">
-        <v>100</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7">
-        <v>20</v>
-      </c>
-      <c r="F7">
-        <v>0.25</v>
-      </c>
-      <c r="G7">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8">
-        <v>70</v>
-      </c>
-      <c r="C8">
-        <v>35</v>
-      </c>
-      <c r="D8">
-        <v>4</v>
-      </c>
-      <c r="E8">
-        <v>10</v>
-      </c>
-      <c r="F8">
-        <v>0.25</v>
-      </c>
-      <c r="G8">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9">
-        <v>100</v>
-      </c>
-      <c r="C9">
-        <v>40</v>
-      </c>
-      <c r="D9">
-        <v>4</v>
-      </c>
-      <c r="E9">
-        <v>15</v>
-      </c>
-      <c r="F9">
-        <v>0.25</v>
-      </c>
-      <c r="G9">
-        <v>0.45</v>
-      </c>
+      <c r="H9" s="2">
+        <v>250</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>